<commit_message>
Inclusão de mais artigos da RBE
</commit_message>
<xml_diff>
--- a/Acompanhamento do download dos artigos.xlsx
+++ b/Acompanhamento do download dos artigos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandresanches/Documents/Projetos/NLP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D829D7-0819-5541-B7C5-A64AB92A4C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBE1B8C-BB24-4E48-8B67-8C5C4674168E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19100" xr2:uid="{8ADA1CC0-93DD-4344-A7A8-A8438D99062B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="6">
   <si>
     <t>OK</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>SEM DADO</t>
+  </si>
+  <si>
+    <t>INCLUIR 0 DEPOIS</t>
+  </si>
+  <si>
+    <t>Todos os artigos do nº 4 são em inglês</t>
   </si>
 </sst>
 </file>
@@ -397,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972CAE1A-9D59-624C-BA29-1EB03ACBB9BE}">
-  <dimension ref="A1:BW5"/>
+  <dimension ref="A1:BW6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="BA2" sqref="BA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -690,6 +696,108 @@
       <c r="S2" t="s">
         <v>0</v>
       </c>
+      <c r="T2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -749,6 +857,108 @@
       <c r="S3" t="s">
         <v>0</v>
       </c>
+      <c r="T3" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -808,6 +1018,108 @@
       <c r="S4" t="s">
         <v>0</v>
       </c>
+      <c r="T4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -866,6 +1178,119 @@
       </c>
       <c r="S5" t="s">
         <v>0</v>
+      </c>
+      <c r="T5" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>0</v>
+      </c>
+      <c r="V5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W5" t="s">
+        <v>0</v>
+      </c>
+      <c r="X5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:75" x14ac:dyDescent="0.2">
+      <c r="AT6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>5</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>